<commit_message>
la page admin marche
</commit_message>
<xml_diff>
--- a/public_html/DOC/Taches.xlsx
+++ b/public_html/DOC/Taches.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -134,13 +134,13 @@
     <t xml:space="preserve">S’accorder sur une palette de couleur</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.13</t>
   </si>
   <si>
     <t xml:space="preserve">Créer style.css commun pour toutes les pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">1.14</t>
@@ -417,6 +417,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,11 +445,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,7 +465,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,7 +553,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -678,9 +678,11 @@
       <c r="F5" s="5" t="n">
         <v>45759</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="9" t="n">
+        <v>45767</v>
+      </c>
       <c r="H5" s="3"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="3" t="s">
         <v>19</v>
       </c>
@@ -698,7 +700,7 @@
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="5" t="n">
         <v>45759</v>
       </c>
@@ -706,10 +708,10 @@
         <v>45760</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -732,10 +734,10 @@
         <v>45761</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="13"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -746,13 +748,13 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5" t="n">
         <v>45759</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K8" s="8"/>
@@ -766,7 +768,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="5" t="n">
         <v>45759</v>
       </c>
@@ -780,9 +782,9 @@
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="5" t="n">
         <v>45759</v>
       </c>
@@ -798,7 +800,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="5" t="n">
         <v>45759</v>
       </c>
@@ -814,7 +816,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="5" t="n">
         <v>45759</v>
       </c>
@@ -830,7 +832,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="14"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="5" t="n">
         <v>45759</v>
       </c>
@@ -846,7 +848,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="5" t="n">
         <v>45759</v>
       </c>
@@ -861,7 +863,9 @@
       <c r="C15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="5" t="n">
         <v>45759</v>
@@ -871,26 +875,29 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="16"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="5" t="n">
         <v>45759</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="16" t="n">
+        <v>45775</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -900,14 +907,17 @@
       <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="5" t="n">
         <v>45759</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="G17" s="16" t="n">
+        <v>45778</v>
+      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -1041,7 +1051,7 @@
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -1051,12 +1061,16 @@
       <c r="C24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="8"/>
       <c r="F24" s="5" t="n">
         <v>45775</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="9" t="n">
+        <v>45777</v>
+      </c>
       <c r="H24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1078,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="5"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1074,7 +1088,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="5"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1162,13 +1176,13 @@
         <v>61</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="6" t="n">
         <v>45776</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,13 +1196,13 @@
         <v>61</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="6" t="n">
         <v>45776</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,13 +1248,13 @@
         <v>61</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="16"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="6" t="n">
         <v>45776</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,13 +1268,13 @@
         <v>61</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="6" t="n">
         <v>45776</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1284,7 @@
       <c r="B37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="18" t="s">
         <v>61</v>
       </c>
       <c r="D37" s="3"/>

</xml_diff>